<commit_message>
gui create, select and run  functions
</commit_message>
<xml_diff>
--- a/get_rif.xlsx
+++ b/get_rif.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
   <si>
     <t xml:space="preserve">RIF</t>
   </si>
@@ -35,9 +35,6 @@
   </si>
   <si>
     <t xml:space="preserve">% RETENCIÓN</t>
-  </si>
-  <si>
-    <t xml:space="preserve">MENSAJE</t>
   </si>
   <si>
     <t xml:space="preserve">INTENTOS</t>
@@ -230,10 +227,10 @@
   <dimension ref="A1:G3"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A3" activeCellId="0" sqref="A3"/>
+      <selection pane="topLeft" activeCell="F22" activeCellId="0" sqref="F22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.640625" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.6796875" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="20.37"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="28.12"/>
@@ -257,16 +254,18 @@
       <c r="E1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="F1" s="1"/>
+      <c r="G1" s="1" t="s">
         <v>5</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>6</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="2"/>
-      <c r="B2" s="2"/>
+      <c r="A2" s="2" t="n">
+        <v>5524325124</v>
+      </c>
+      <c r="B2" s="2" t="n">
+        <v>233342</v>
+      </c>
     </row>
     <row r="3" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="2"/>

</xml_diff>